<commit_message>
secon file with more compact code in functions
</commit_message>
<xml_diff>
--- a/RandomForest_output.xlsx
+++ b/RandomForest_output.xlsx
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>421.1508333333333</v>
+        <v>421.1508333333334</v>
       </c>
     </row>
     <row r="7">
@@ -501,7 +501,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>284.4251666666665</v>
+        <v>284.4251666666666</v>
       </c>
     </row>
     <row r="10">
@@ -533,7 +533,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="14">
@@ -597,7 +597,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>363.7166666666667</v>
+        <v>363.7166666666666</v>
       </c>
     </row>
     <row r="22">
@@ -661,7 +661,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>292.5783888888887</v>
+        <v>292.5783888888888</v>
       </c>
     </row>
     <row r="30">
@@ -749,7 +749,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>1615.281166666667</v>
+        <v>1615.281166666666</v>
       </c>
     </row>
     <row r="41">
@@ -805,7 +805,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>302.9873333333333</v>
+        <v>302.9873333333334</v>
       </c>
     </row>
     <row r="48">
@@ -941,7 +941,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>332.3634999999999</v>
+        <v>332.3635</v>
       </c>
     </row>
     <row r="65">
@@ -1005,7 +1005,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>361.174</v>
+        <v>361.1740000000001</v>
       </c>
     </row>
     <row r="73">
@@ -1053,7 +1053,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="79">
@@ -1285,7 +1285,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>555.3027777777777</v>
+        <v>555.3027777777778</v>
       </c>
     </row>
     <row r="108">
@@ -1317,7 +1317,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>555.3027777777777</v>
+        <v>555.3027777777778</v>
       </c>
     </row>
     <row r="112">
@@ -1389,7 +1389,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>639.6166666666666</v>
+        <v>639.6166666666667</v>
       </c>
     </row>
     <row r="121">
@@ -1557,7 +1557,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>417.4206428571428</v>
+        <v>417.4206428571429</v>
       </c>
     </row>
     <row r="142">
@@ -1589,7 +1589,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>263.95</v>
+        <v>263.9500000000001</v>
       </c>
     </row>
     <row r="146">
@@ -1653,7 +1653,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>213.1833333333333</v>
+        <v>213.1833333333334</v>
       </c>
     </row>
     <row r="154">
@@ -1709,7 +1709,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>336.2792222222224</v>
+        <v>336.2792222222223</v>
       </c>
     </row>
     <row r="161">
@@ -1725,7 +1725,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>356.4346666666665</v>
+        <v>356.4346666666666</v>
       </c>
     </row>
     <row r="163">
@@ -1757,7 +1757,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>776.4400833333334</v>
+        <v>776.4400833333335</v>
       </c>
     </row>
     <row r="167">
@@ -1797,7 +1797,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>281.5266666666667</v>
+        <v>281.5266666666666</v>
       </c>
     </row>
     <row r="172">
@@ -1813,7 +1813,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>270.2802222222223</v>
+        <v>270.2802222222222</v>
       </c>
     </row>
     <row r="174">
@@ -1837,7 +1837,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>735.1555555555556</v>
+        <v>735.1555555555557</v>
       </c>
     </row>
     <row r="177">
@@ -1981,7 +1981,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>352.375</v>
+        <v>352.3750000000001</v>
       </c>
     </row>
     <row r="195">
@@ -1989,7 +1989,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>754.7140000000001</v>
+        <v>754.7139999999999</v>
       </c>
     </row>
     <row r="196">
@@ -2125,7 +2125,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>701.4834999999999</v>
+        <v>701.4834999999998</v>
       </c>
     </row>
     <row r="213">
@@ -2197,7 +2197,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>294.1</v>
+        <v>294.1000000000001</v>
       </c>
     </row>
     <row r="222">
@@ -2277,7 +2277,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>448.745</v>
+        <v>448.7450000000001</v>
       </c>
     </row>
     <row r="232">
@@ -2293,7 +2293,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>302.1614444444447</v>
+        <v>302.1614444444446</v>
       </c>
     </row>
     <row r="234">
@@ -2309,7 +2309,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>313.6253333333333</v>
+        <v>313.6253333333334</v>
       </c>
     </row>
     <row r="236">
@@ -2493,7 +2493,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>398.9393333333332</v>
+        <v>398.9393333333333</v>
       </c>
     </row>
     <row r="259">
@@ -2581,7 +2581,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="n">
-        <v>339.2967380952382</v>
+        <v>339.2967380952381</v>
       </c>
     </row>
     <row r="270">
@@ -2653,7 +2653,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="n">
-        <v>802.7666666666668</v>
+        <v>802.7666666666667</v>
       </c>
     </row>
     <row r="279">
@@ -2693,7 +2693,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="n">
-        <v>212.9896666666666</v>
+        <v>212.9896666666665</v>
       </c>
     </row>
     <row r="284">
@@ -2933,7 +2933,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="n">
-        <v>930.7769666666666</v>
+        <v>930.7769666666667</v>
       </c>
     </row>
     <row r="314">
@@ -2989,7 +2989,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="n">
-        <v>472.3176666666667</v>
+        <v>472.3176666666666</v>
       </c>
     </row>
     <row r="321">
@@ -2997,7 +2997,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="n">
-        <v>252.5277777777777</v>
+        <v>252.5277777777778</v>
       </c>
     </row>
     <row r="322">
@@ -3069,7 +3069,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="n">
-        <v>983.1904444444444</v>
+        <v>983.1904444444447</v>
       </c>
     </row>
     <row r="331">
@@ -3117,7 +3117,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="n">
-        <v>378.8299999999999</v>
+        <v>378.83</v>
       </c>
     </row>
     <row r="337">
@@ -3189,7 +3189,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="n">
-        <v>238.7333333333335</v>
+        <v>238.7333333333334</v>
       </c>
     </row>
     <row r="346">
@@ -3197,7 +3197,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="n">
-        <v>272.3881666666666</v>
+        <v>272.3881666666665</v>
       </c>
     </row>
     <row r="347">
@@ -3237,7 +3237,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="n">
-        <v>253.9428611111111</v>
+        <v>253.942861111111</v>
       </c>
     </row>
     <row r="352">
@@ -3325,7 +3325,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="n">
-        <v>925.4279999999999</v>
+        <v>925.4280000000001</v>
       </c>
     </row>
     <row r="363">
@@ -3389,7 +3389,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>757.5124999999999</v>
+        <v>757.5125</v>
       </c>
     </row>
     <row r="371">
@@ -3445,7 +3445,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="n">
-        <v>389.4313333333333</v>
+        <v>389.4313333333334</v>
       </c>
     </row>
     <row r="378">
@@ -3477,7 +3477,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>2694.713305555555</v>
+        <v>2694.713305555554</v>
       </c>
     </row>
     <row r="382">
@@ -3525,7 +3525,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="n">
-        <v>418.2546666666666</v>
+        <v>418.2546666666667</v>
       </c>
     </row>
     <row r="388">
@@ -3533,7 +3533,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="n">
-        <v>718.7467128205128</v>
+        <v>718.7467128205127</v>
       </c>
     </row>
     <row r="389">
@@ -3541,7 +3541,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="390">
@@ -3557,7 +3557,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="n">
-        <v>466.5451666666667</v>
+        <v>466.5451666666666</v>
       </c>
     </row>
     <row r="392">
@@ -3669,7 +3669,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="n">
-        <v>654.7166666666666</v>
+        <v>654.7166666666665</v>
       </c>
     </row>
     <row r="406">
@@ -3701,7 +3701,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="n">
-        <v>569.4416666666666</v>
+        <v>569.4416666666667</v>
       </c>
     </row>
     <row r="410">
@@ -3805,7 +3805,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="n">
-        <v>499.5966666666666</v>
+        <v>499.5966666666667</v>
       </c>
     </row>
     <row r="423">
@@ -3853,7 +3853,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="n">
-        <v>342.8926111111111</v>
+        <v>342.8926111111112</v>
       </c>
     </row>
     <row r="429">
@@ -3861,7 +3861,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="n">
-        <v>365.1703333333333</v>
+        <v>365.1703333333332</v>
       </c>
     </row>
     <row r="430">
@@ -3877,7 +3877,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="n">
-        <v>962.7798333333334</v>
+        <v>962.7798333333333</v>
       </c>
     </row>
     <row r="432">
@@ -3957,7 +3957,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="n">
-        <v>366.2572222222223</v>
+        <v>366.2572222222222</v>
       </c>
     </row>
     <row r="442">
@@ -3981,7 +3981,7 @@
         <v>442</v>
       </c>
       <c r="B444" t="n">
-        <v>194.2123333333334</v>
+        <v>194.2123333333333</v>
       </c>
     </row>
     <row r="445">
@@ -3989,7 +3989,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="n">
-        <v>391.089</v>
+        <v>391.0890000000001</v>
       </c>
     </row>
     <row r="446">
@@ -4053,7 +4053,7 @@
         <v>451</v>
       </c>
       <c r="B453" t="n">
-        <v>217.109</v>
+        <v>217.1090000000002</v>
       </c>
     </row>
     <row r="454">
@@ -4181,7 +4181,7 @@
         <v>467</v>
       </c>
       <c r="B469" t="n">
-        <v>278.6770833333333</v>
+        <v>278.6770833333332</v>
       </c>
     </row>
     <row r="470">
@@ -4349,7 +4349,7 @@
         <v>488</v>
       </c>
       <c r="B490" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="491">
@@ -4453,7 +4453,7 @@
         <v>501</v>
       </c>
       <c r="B503" t="n">
-        <v>280.4</v>
+        <v>280.4000000000001</v>
       </c>
     </row>
     <row r="504">
@@ -4517,7 +4517,7 @@
         <v>509</v>
       </c>
       <c r="B511" t="n">
-        <v>291.6779999999998</v>
+        <v>291.6779999999999</v>
       </c>
     </row>
     <row r="512">
@@ -4605,7 +4605,7 @@
         <v>520</v>
       </c>
       <c r="B522" t="n">
-        <v>353.9449999999999</v>
+        <v>353.9450000000001</v>
       </c>
     </row>
     <row r="523">
@@ -4637,7 +4637,7 @@
         <v>524</v>
       </c>
       <c r="B526" t="n">
-        <v>163.0833333333332</v>
+        <v>163.0833333333333</v>
       </c>
     </row>
     <row r="527">
@@ -4765,7 +4765,7 @@
         <v>540</v>
       </c>
       <c r="B542" t="n">
-        <v>395.875</v>
+        <v>395.8749999999999</v>
       </c>
     </row>
     <row r="543">
@@ -4773,7 +4773,7 @@
         <v>541</v>
       </c>
       <c r="B543" t="n">
-        <v>855.1602999999999</v>
+        <v>855.1602999999998</v>
       </c>
     </row>
     <row r="544">
@@ -4821,7 +4821,7 @@
         <v>547</v>
       </c>
       <c r="B549" t="n">
-        <v>361.965</v>
+        <v>361.9649999999999</v>
       </c>
     </row>
     <row r="550">
@@ -4893,7 +4893,7 @@
         <v>556</v>
       </c>
       <c r="B558" t="n">
-        <v>430.7</v>
+        <v>430.6999999999999</v>
       </c>
     </row>
     <row r="559">
@@ -4981,7 +4981,7 @@
         <v>567</v>
       </c>
       <c r="B569" t="n">
-        <v>266.6513333333334</v>
+        <v>266.6513333333335</v>
       </c>
     </row>
     <row r="570">
@@ -5045,7 +5045,7 @@
         <v>575</v>
       </c>
       <c r="B577" t="n">
-        <v>421.8166666666667</v>
+        <v>421.8166666666666</v>
       </c>
     </row>
     <row r="578">
@@ -5213,7 +5213,7 @@
         <v>596</v>
       </c>
       <c r="B598" t="n">
-        <v>154.9333333333333</v>
+        <v>154.9333333333334</v>
       </c>
     </row>
     <row r="599">
@@ -5277,7 +5277,7 @@
         <v>604</v>
       </c>
       <c r="B606" t="n">
-        <v>283.7619999999999</v>
+        <v>283.7619999999998</v>
       </c>
     </row>
     <row r="607">
@@ -5309,7 +5309,7 @@
         <v>608</v>
       </c>
       <c r="B610" t="n">
-        <v>305.3105555555555</v>
+        <v>305.3105555555556</v>
       </c>
     </row>
     <row r="611">
@@ -5445,7 +5445,7 @@
         <v>625</v>
       </c>
       <c r="B627" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="628">
@@ -5493,7 +5493,7 @@
         <v>631</v>
       </c>
       <c r="B633" t="n">
-        <v>712.6983333333333</v>
+        <v>712.6983333333334</v>
       </c>
     </row>
     <row r="634">
@@ -5525,7 +5525,7 @@
         <v>635</v>
       </c>
       <c r="B637" t="n">
-        <v>333.9616666666667</v>
+        <v>333.9616666666668</v>
       </c>
     </row>
     <row r="638">
@@ -5581,7 +5581,7 @@
         <v>642</v>
       </c>
       <c r="B644" t="n">
-        <v>559.0186666666667</v>
+        <v>559.0186666666666</v>
       </c>
     </row>
     <row r="645">
@@ -5733,7 +5733,7 @@
         <v>661</v>
       </c>
       <c r="B663" t="n">
-        <v>267.7466666666666</v>
+        <v>267.7466666666665</v>
       </c>
     </row>
     <row r="664">
@@ -5813,7 +5813,7 @@
         <v>671</v>
       </c>
       <c r="B673" t="n">
-        <v>314.356</v>
+        <v>314.3560000000001</v>
       </c>
     </row>
     <row r="674">
@@ -5821,7 +5821,7 @@
         <v>672</v>
       </c>
       <c r="B674" t="n">
-        <v>404.7266666666667</v>
+        <v>404.7266666666666</v>
       </c>
     </row>
     <row r="675">
@@ -5877,7 +5877,7 @@
         <v>679</v>
       </c>
       <c r="B681" t="n">
-        <v>845.6666666666666</v>
+        <v>845.6666666666667</v>
       </c>
     </row>
     <row r="682">
@@ -5901,7 +5901,7 @@
         <v>682</v>
       </c>
       <c r="B684" t="n">
-        <v>689.3325833333333</v>
+        <v>689.3325833333332</v>
       </c>
     </row>
     <row r="685">
@@ -5933,7 +5933,7 @@
         <v>686</v>
       </c>
       <c r="B688" t="n">
-        <v>315.7807478632479</v>
+        <v>315.7807478632478</v>
       </c>
     </row>
     <row r="689">
@@ -6005,7 +6005,7 @@
         <v>695</v>
       </c>
       <c r="B697" t="n">
-        <v>716.0944444444443</v>
+        <v>716.0944444444444</v>
       </c>
     </row>
     <row r="698">
@@ -6061,7 +6061,7 @@
         <v>702</v>
       </c>
       <c r="B704" t="n">
-        <v>602.3943333333333</v>
+        <v>602.3943333333334</v>
       </c>
     </row>
     <row r="705">
@@ -6069,7 +6069,7 @@
         <v>703</v>
       </c>
       <c r="B705" t="n">
-        <v>2384.378688888889</v>
+        <v>2384.378688888888</v>
       </c>
     </row>
     <row r="706">
@@ -6125,7 +6125,7 @@
         <v>710</v>
       </c>
       <c r="B712" t="n">
-        <v>433.9722916666666</v>
+        <v>433.9722916666667</v>
       </c>
     </row>
     <row r="713">
@@ -6149,7 +6149,7 @@
         <v>713</v>
       </c>
       <c r="B715" t="n">
-        <v>527.0433333333333</v>
+        <v>527.0433333333334</v>
       </c>
     </row>
     <row r="716">
@@ -6277,7 +6277,7 @@
         <v>729</v>
       </c>
       <c r="B731" t="n">
-        <v>215.9999999999999</v>
+        <v>216</v>
       </c>
     </row>
     <row r="732">
@@ -6373,7 +6373,7 @@
         <v>741</v>
       </c>
       <c r="B743" t="n">
-        <v>291.9166666666666</v>
+        <v>291.9166666666665</v>
       </c>
     </row>
     <row r="744">
@@ -6389,7 +6389,7 @@
         <v>743</v>
       </c>
       <c r="B745" t="n">
-        <v>287.6666666666666</v>
+        <v>287.6666666666665</v>
       </c>
     </row>
     <row r="746">
@@ -6429,7 +6429,7 @@
         <v>748</v>
       </c>
       <c r="B750" t="n">
-        <v>262.5848333333334</v>
+        <v>262.5848333333333</v>
       </c>
     </row>
     <row r="751">
@@ -6501,7 +6501,7 @@
         <v>757</v>
       </c>
       <c r="B759" t="n">
-        <v>3930.480666666664</v>
+        <v>3930.480666666665</v>
       </c>
     </row>
     <row r="760">
@@ -6589,7 +6589,7 @@
         <v>768</v>
       </c>
       <c r="B770" t="n">
-        <v>789.5781999999999</v>
+        <v>789.5782</v>
       </c>
     </row>
     <row r="771">
@@ -6597,7 +6597,7 @@
         <v>769</v>
       </c>
       <c r="B771" t="n">
-        <v>266.1714999999999</v>
+        <v>266.1715</v>
       </c>
     </row>
     <row r="772">
@@ -6605,7 +6605,7 @@
         <v>770</v>
       </c>
       <c r="B772" t="n">
-        <v>431.3718333333334</v>
+        <v>431.3718333333333</v>
       </c>
     </row>
     <row r="773">
@@ -6637,7 +6637,7 @@
         <v>774</v>
       </c>
       <c r="B776" t="n">
-        <v>637.556</v>
+        <v>637.5559999999999</v>
       </c>
     </row>
     <row r="777">
@@ -6661,7 +6661,7 @@
         <v>777</v>
       </c>
       <c r="B779" t="n">
-        <v>419.9906666666666</v>
+        <v>419.9906666666665</v>
       </c>
     </row>
     <row r="780">
@@ -6717,7 +6717,7 @@
         <v>784</v>
       </c>
       <c r="B786" t="n">
-        <v>548.704</v>
+        <v>548.7040000000001</v>
       </c>
     </row>
     <row r="787">
@@ -6725,7 +6725,7 @@
         <v>785</v>
       </c>
       <c r="B787" t="n">
-        <v>254.8903333333334</v>
+        <v>254.8903333333335</v>
       </c>
     </row>
     <row r="788">
@@ -6797,7 +6797,7 @@
         <v>794</v>
       </c>
       <c r="B796" t="n">
-        <v>178.9166666666666</v>
+        <v>178.9166666666667</v>
       </c>
     </row>
     <row r="797">
@@ -6877,7 +6877,7 @@
         <v>804</v>
       </c>
       <c r="B806" t="n">
-        <v>415.8284166666667</v>
+        <v>415.8284166666666</v>
       </c>
     </row>
     <row r="807">
@@ -6933,7 +6933,7 @@
         <v>811</v>
       </c>
       <c r="B813" t="n">
-        <v>794.083333333333</v>
+        <v>794.0833333333331</v>
       </c>
     </row>
     <row r="814">
@@ -6941,7 +6941,7 @@
         <v>812</v>
       </c>
       <c r="B814" t="n">
-        <v>273.1166666666667</v>
+        <v>273.1166666666666</v>
       </c>
     </row>
     <row r="815">
@@ -6957,7 +6957,7 @@
         <v>814</v>
       </c>
       <c r="B816" t="n">
-        <v>328.721</v>
+        <v>328.7209999999999</v>
       </c>
     </row>
     <row r="817">
@@ -6981,7 +6981,7 @@
         <v>817</v>
       </c>
       <c r="B819" t="n">
-        <v>705.9050777777777</v>
+        <v>705.9050777777778</v>
       </c>
     </row>
     <row r="820">
@@ -7013,7 +7013,7 @@
         <v>821</v>
       </c>
       <c r="B823" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="824">
@@ -7029,7 +7029,7 @@
         <v>823</v>
       </c>
       <c r="B825" t="n">
-        <v>312.7297142857143</v>
+        <v>312.7297142857142</v>
       </c>
     </row>
     <row r="826">
@@ -7149,7 +7149,7 @@
         <v>838</v>
       </c>
       <c r="B840" t="n">
-        <v>2265.34925</v>
+        <v>2265.349249999999</v>
       </c>
     </row>
     <row r="841">
@@ -7197,7 +7197,7 @@
         <v>844</v>
       </c>
       <c r="B846" t="n">
-        <v>399.5616666666666</v>
+        <v>399.5616666666667</v>
       </c>
     </row>
     <row r="847">
@@ -7213,7 +7213,7 @@
         <v>846</v>
       </c>
       <c r="B848" t="n">
-        <v>824.3022111111111</v>
+        <v>824.302211111111</v>
       </c>
     </row>
     <row r="849">
@@ -7285,7 +7285,7 @@
         <v>855</v>
       </c>
       <c r="B857" t="n">
-        <v>367.0951666666667</v>
+        <v>367.0951666666666</v>
       </c>
     </row>
     <row r="858">
@@ -7293,7 +7293,7 @@
         <v>856</v>
       </c>
       <c r="B858" t="n">
-        <v>176.1055555555554</v>
+        <v>176.1055555555555</v>
       </c>
     </row>
     <row r="859">
@@ -7309,7 +7309,7 @@
         <v>858</v>
       </c>
       <c r="B860" t="n">
-        <v>305.6833333333332</v>
+        <v>305.6833333333333</v>
       </c>
     </row>
     <row r="861">
@@ -7341,7 +7341,7 @@
         <v>862</v>
       </c>
       <c r="B864" t="n">
-        <v>757.6485194444442</v>
+        <v>757.6485194444444</v>
       </c>
     </row>
     <row r="865">
@@ -7485,7 +7485,7 @@
         <v>880</v>
       </c>
       <c r="B882" t="n">
-        <v>388.6979999999999</v>
+        <v>388.698</v>
       </c>
     </row>
     <row r="883">
@@ -7533,7 +7533,7 @@
         <v>886</v>
       </c>
       <c r="B888" t="n">
-        <v>453.678</v>
+        <v>453.6779999999999</v>
       </c>
     </row>
     <row r="889">
@@ -7581,7 +7581,7 @@
         <v>892</v>
       </c>
       <c r="B894" t="n">
-        <v>373.411</v>
+        <v>373.4109999999999</v>
       </c>
     </row>
     <row r="895">
@@ -7749,7 +7749,7 @@
         <v>913</v>
       </c>
       <c r="B915" t="n">
-        <v>654.3753333333333</v>
+        <v>654.3753333333334</v>
       </c>
     </row>
     <row r="916">
@@ -7917,7 +7917,7 @@
         <v>934</v>
       </c>
       <c r="B936" t="n">
-        <v>126.5000000000002</v>
+        <v>126.5000000000001</v>
       </c>
     </row>
     <row r="937">
@@ -7973,7 +7973,7 @@
         <v>941</v>
       </c>
       <c r="B943" t="n">
-        <v>275.8955</v>
+        <v>275.8955000000001</v>
       </c>
     </row>
     <row r="944">
@@ -7981,7 +7981,7 @@
         <v>942</v>
       </c>
       <c r="B944" t="n">
-        <v>378.1833333333334</v>
+        <v>378.1833333333333</v>
       </c>
     </row>
     <row r="945">
@@ -8021,7 +8021,7 @@
         <v>947</v>
       </c>
       <c r="B949" t="n">
-        <v>542.6560000000001</v>
+        <v>542.6559999999999</v>
       </c>
     </row>
     <row r="950">
@@ -8029,7 +8029,7 @@
         <v>948</v>
       </c>
       <c r="B950" t="n">
-        <v>251.4394444444444</v>
+        <v>251.4394444444443</v>
       </c>
     </row>
     <row r="951">
@@ -8085,7 +8085,7 @@
         <v>955</v>
       </c>
       <c r="B957" t="n">
-        <v>195.4363333333336</v>
+        <v>195.4363333333337</v>
       </c>
     </row>
     <row r="958">
@@ -8133,7 +8133,7 @@
         <v>961</v>
       </c>
       <c r="B963" t="n">
-        <v>325.5766666666668</v>
+        <v>325.5766666666667</v>
       </c>
     </row>
     <row r="964">
@@ -8197,7 +8197,7 @@
         <v>969</v>
       </c>
       <c r="B971" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="972">
@@ -8205,7 +8205,7 @@
         <v>970</v>
       </c>
       <c r="B972" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="973">
@@ -8237,7 +8237,7 @@
         <v>974</v>
       </c>
       <c r="B976" t="n">
-        <v>298.3095833333333</v>
+        <v>298.3095833333332</v>
       </c>
     </row>
     <row r="977">
@@ -8253,7 +8253,7 @@
         <v>976</v>
       </c>
       <c r="B978" t="n">
-        <v>442.4360000000001</v>
+        <v>442.436</v>
       </c>
     </row>
     <row r="979">
@@ -8301,7 +8301,7 @@
         <v>982</v>
       </c>
       <c r="B984" t="n">
-        <v>226.6858333333334</v>
+        <v>226.6858333333335</v>
       </c>
     </row>
     <row r="985">
@@ -8429,7 +8429,7 @@
         <v>998</v>
       </c>
       <c r="B1000" t="n">
-        <v>317.7341666666665</v>
+        <v>317.7341666666666</v>
       </c>
     </row>
     <row r="1001">
@@ -8453,7 +8453,7 @@
         <v>1001</v>
       </c>
       <c r="B1003" t="n">
-        <v>251.2658333333333</v>
+        <v>251.2658333333334</v>
       </c>
     </row>
     <row r="1004">
@@ -8533,7 +8533,7 @@
         <v>1011</v>
       </c>
       <c r="B1013" t="n">
-        <v>918.3457444444443</v>
+        <v>918.3457444444446</v>
       </c>
     </row>
     <row r="1014">
@@ -8573,7 +8573,7 @@
         <v>1016</v>
       </c>
       <c r="B1018" t="n">
-        <v>232.6649999999998</v>
+        <v>232.6649999999999</v>
       </c>
     </row>
     <row r="1019">
@@ -8605,7 +8605,7 @@
         <v>1020</v>
       </c>
       <c r="B1022" t="n">
-        <v>326.2381666666668</v>
+        <v>326.2381666666666</v>
       </c>
     </row>
     <row r="1023">
@@ -8613,7 +8613,7 @@
         <v>1021</v>
       </c>
       <c r="B1023" t="n">
-        <v>238.786</v>
+        <v>238.7859999999999</v>
       </c>
     </row>
     <row r="1024">
@@ -8637,7 +8637,7 @@
         <v>1024</v>
       </c>
       <c r="B1026" t="n">
-        <v>364.4366666666667</v>
+        <v>364.4366666666666</v>
       </c>
     </row>
     <row r="1027">
@@ -8669,7 +8669,7 @@
         <v>1028</v>
       </c>
       <c r="B1030" t="n">
-        <v>434.0956944444445</v>
+        <v>434.0956944444444</v>
       </c>
     </row>
     <row r="1031">
@@ -8765,7 +8765,7 @@
         <v>1040</v>
       </c>
       <c r="B1042" t="n">
-        <v>356.4189444444445</v>
+        <v>356.4189444444444</v>
       </c>
     </row>
     <row r="1043">
@@ -8869,7 +8869,7 @@
         <v>1053</v>
       </c>
       <c r="B1055" t="n">
-        <v>318.0863333333333</v>
+        <v>318.0863333333332</v>
       </c>
     </row>
     <row r="1056">
@@ -9101,7 +9101,7 @@
         <v>1082</v>
       </c>
       <c r="B1084" t="n">
-        <v>525.2926666666666</v>
+        <v>525.2926666666667</v>
       </c>
     </row>
     <row r="1085">
@@ -9109,7 +9109,7 @@
         <v>1083</v>
       </c>
       <c r="B1085" t="n">
-        <v>322.25</v>
+        <v>322.2499999999999</v>
       </c>
     </row>
     <row r="1086">
@@ -9141,7 +9141,7 @@
         <v>1087</v>
       </c>
       <c r="B1089" t="n">
-        <v>348.6979166666667</v>
+        <v>348.6979166666666</v>
       </c>
     </row>
     <row r="1090">
@@ -9237,7 +9237,7 @@
         <v>1099</v>
       </c>
       <c r="B1101" t="n">
-        <v>923.0166666666665</v>
+        <v>923.0166666666667</v>
       </c>
     </row>
     <row r="1102">
@@ -9261,7 +9261,7 @@
         <v>1102</v>
       </c>
       <c r="B1104" t="n">
-        <v>1045.445333333334</v>
+        <v>1045.445333333333</v>
       </c>
     </row>
     <row r="1105">
@@ -9381,7 +9381,7 @@
         <v>1117</v>
       </c>
       <c r="B1119" t="n">
-        <v>318.5979999999999</v>
+        <v>318.598</v>
       </c>
     </row>
     <row r="1120">
@@ -9517,7 +9517,7 @@
         <v>1134</v>
       </c>
       <c r="B1136" t="n">
-        <v>998.6701666666667</v>
+        <v>998.6701666666668</v>
       </c>
     </row>
     <row r="1137">
@@ -9573,7 +9573,7 @@
         <v>1141</v>
       </c>
       <c r="B1143" t="n">
-        <v>827.6162777777777</v>
+        <v>827.6162777777778</v>
       </c>
     </row>
     <row r="1144">
@@ -9605,7 +9605,7 @@
         <v>1145</v>
       </c>
       <c r="B1147" t="n">
-        <v>332.8523015873015</v>
+        <v>332.8523015873016</v>
       </c>
     </row>
     <row r="1148">
@@ -9661,7 +9661,7 @@
         <v>1152</v>
       </c>
       <c r="B1154" t="n">
-        <v>556.8050000000001</v>
+        <v>556.8049999999999</v>
       </c>
     </row>
     <row r="1155">
@@ -9725,7 +9725,7 @@
         <v>1160</v>
       </c>
       <c r="B1162" t="n">
-        <v>432.4166666666666</v>
+        <v>432.4166666666667</v>
       </c>
     </row>
     <row r="1163">
@@ -9741,7 +9741,7 @@
         <v>1162</v>
       </c>
       <c r="B1164" t="n">
-        <v>439.7236666666666</v>
+        <v>439.7236666666667</v>
       </c>
     </row>
     <row r="1165">
@@ -9805,7 +9805,7 @@
         <v>1170</v>
       </c>
       <c r="B1172" t="n">
-        <v>387.7425</v>
+        <v>387.7424999999999</v>
       </c>
     </row>
     <row r="1173">
@@ -9829,7 +9829,7 @@
         <v>1173</v>
       </c>
       <c r="B1175" t="n">
-        <v>277.9215</v>
+        <v>277.9214999999999</v>
       </c>
     </row>
     <row r="1176">
@@ -9853,7 +9853,7 @@
         <v>1176</v>
       </c>
       <c r="B1178" t="n">
-        <v>302.3151666666666</v>
+        <v>302.3151666666667</v>
       </c>
     </row>
     <row r="1179">
@@ -9909,7 +9909,7 @@
         <v>1183</v>
       </c>
       <c r="B1185" t="n">
-        <v>279.4540000000002</v>
+        <v>279.4540000000001</v>
       </c>
     </row>
     <row r="1186">
@@ -10013,7 +10013,7 @@
         <v>1196</v>
       </c>
       <c r="B1198" t="n">
-        <v>711.0976666666668</v>
+        <v>711.0976666666667</v>
       </c>
     </row>
     <row r="1199">
@@ -10061,7 +10061,7 @@
         <v>1202</v>
       </c>
       <c r="B1204" t="n">
-        <v>132.6000000000001</v>
+        <v>132.6</v>
       </c>
     </row>
     <row r="1205">
@@ -10085,7 +10085,7 @@
         <v>1205</v>
       </c>
       <c r="B1207" t="n">
-        <v>296.4166666666667</v>
+        <v>296.4166666666666</v>
       </c>
     </row>
     <row r="1208">
@@ -10125,7 +10125,7 @@
         <v>1210</v>
       </c>
       <c r="B1212" t="n">
-        <v>676.4836666666667</v>
+        <v>676.4836666666666</v>
       </c>
     </row>
     <row r="1213">
@@ -10189,7 +10189,7 @@
         <v>1218</v>
       </c>
       <c r="B1220" t="n">
-        <v>489.9517777777778</v>
+        <v>489.9517777777777</v>
       </c>
     </row>
     <row r="1221">
@@ -10205,7 +10205,7 @@
         <v>1220</v>
       </c>
       <c r="B1222" t="n">
-        <v>282.4249999999998</v>
+        <v>282.425</v>
       </c>
     </row>
     <row r="1223">
@@ -10269,7 +10269,7 @@
         <v>1228</v>
       </c>
       <c r="B1230" t="n">
-        <v>329.9805555555557</v>
+        <v>329.9805555555556</v>
       </c>
     </row>
     <row r="1231">
@@ -10277,7 +10277,7 @@
         <v>1229</v>
       </c>
       <c r="B1231" t="n">
-        <v>332.1575277777778</v>
+        <v>332.1575277777779</v>
       </c>
     </row>
     <row r="1232">
@@ -10309,7 +10309,7 @@
         <v>1233</v>
       </c>
       <c r="B1235" t="n">
-        <v>456.4719999999999</v>
+        <v>456.472</v>
       </c>
     </row>
     <row r="1236">
@@ -10349,7 +10349,7 @@
         <v>1238</v>
       </c>
       <c r="B1240" t="n">
-        <v>329.7753333333333</v>
+        <v>329.7753333333334</v>
       </c>
     </row>
     <row r="1241">
@@ -10373,7 +10373,7 @@
         <v>1241</v>
       </c>
       <c r="B1243" t="n">
-        <v>309.3708333333334</v>
+        <v>309.3708333333333</v>
       </c>
     </row>
     <row r="1244">
@@ -10397,7 +10397,7 @@
         <v>1244</v>
       </c>
       <c r="B1246" t="n">
-        <v>361.3418333333334</v>
+        <v>361.3418333333333</v>
       </c>
     </row>
     <row r="1247">
@@ -10485,7 +10485,7 @@
         <v>1255</v>
       </c>
       <c r="B1257" t="n">
-        <v>493.8283333333333</v>
+        <v>493.8283333333334</v>
       </c>
     </row>
     <row r="1258">
@@ -10541,7 +10541,7 @@
         <v>1262</v>
       </c>
       <c r="B1264" t="n">
-        <v>474.6813648148148</v>
+        <v>474.6813648148147</v>
       </c>
     </row>
     <row r="1265">
@@ -10549,7 +10549,7 @@
         <v>1263</v>
       </c>
       <c r="B1265" t="n">
-        <v>757.7146666666665</v>
+        <v>757.7146666666666</v>
       </c>
     </row>
     <row r="1266">
@@ -10565,7 +10565,7 @@
         <v>1265</v>
       </c>
       <c r="B1267" t="n">
-        <v>329.3993333333333</v>
+        <v>329.3993333333332</v>
       </c>
     </row>
     <row r="1268">
@@ -10597,7 +10597,7 @@
         <v>1269</v>
       </c>
       <c r="B1271" t="n">
-        <v>781.5553888888887</v>
+        <v>781.5553888888888</v>
       </c>
     </row>
     <row r="1272">
@@ -10605,7 +10605,7 @@
         <v>1270</v>
       </c>
       <c r="B1272" t="n">
-        <v>541.3938611111112</v>
+        <v>541.3938611111111</v>
       </c>
     </row>
     <row r="1273">
@@ -10613,7 +10613,7 @@
         <v>1271</v>
       </c>
       <c r="B1273" t="n">
-        <v>285.7833333333333</v>
+        <v>285.7833333333334</v>
       </c>
     </row>
     <row r="1274">
@@ -10733,7 +10733,7 @@
         <v>1286</v>
       </c>
       <c r="B1288" t="n">
-        <v>319.2548333333334</v>
+        <v>319.2548333333335</v>
       </c>
     </row>
     <row r="1289">
@@ -10749,7 +10749,7 @@
         <v>1288</v>
       </c>
       <c r="B1290" t="n">
-        <v>407.8099999999999</v>
+        <v>407.8100000000001</v>
       </c>
     </row>
     <row r="1291">
@@ -10781,7 +10781,7 @@
         <v>1292</v>
       </c>
       <c r="B1294" t="n">
-        <v>411.0363235294118</v>
+        <v>411.0363235294119</v>
       </c>
     </row>
     <row r="1295">
@@ -11005,7 +11005,7 @@
         <v>1320</v>
       </c>
       <c r="B1322" t="n">
-        <v>298.1111111111111</v>
+        <v>298.111111111111</v>
       </c>
     </row>
     <row r="1323">
@@ -11013,7 +11013,7 @@
         <v>1321</v>
       </c>
       <c r="B1323" t="n">
-        <v>354.1810555555554</v>
+        <v>354.1810555555555</v>
       </c>
     </row>
     <row r="1324">
@@ -11029,7 +11029,7 @@
         <v>1323</v>
       </c>
       <c r="B1325" t="n">
-        <v>774.0946666666666</v>
+        <v>774.0946666666667</v>
       </c>
     </row>
     <row r="1326">
@@ -11045,7 +11045,7 @@
         <v>1325</v>
       </c>
       <c r="B1327" t="n">
-        <v>385.7215000000001</v>
+        <v>385.7215</v>
       </c>
     </row>
     <row r="1328">
@@ -11085,7 +11085,7 @@
         <v>1330</v>
       </c>
       <c r="B1332" t="n">
-        <v>330.1895</v>
+        <v>330.1894999999999</v>
       </c>
     </row>
     <row r="1333">
@@ -11125,7 +11125,7 @@
         <v>1335</v>
       </c>
       <c r="B1337" t="n">
-        <v>239.0333333333334</v>
+        <v>239.0333333333335</v>
       </c>
     </row>
     <row r="1338">
@@ -11157,7 +11157,7 @@
         <v>1339</v>
       </c>
       <c r="B1341" t="n">
-        <v>363.6678333333332</v>
+        <v>363.6678333333333</v>
       </c>
     </row>
     <row r="1342">
@@ -11205,7 +11205,7 @@
         <v>1345</v>
       </c>
       <c r="B1347" t="n">
-        <v>391.5696111111112</v>
+        <v>391.5696111111111</v>
       </c>
     </row>
     <row r="1348">
@@ -11269,7 +11269,7 @@
         <v>1353</v>
       </c>
       <c r="B1355" t="n">
-        <v>710.3866666666667</v>
+        <v>710.3866666666665</v>
       </c>
     </row>
     <row r="1356">
@@ -11301,7 +11301,7 @@
         <v>1357</v>
       </c>
       <c r="B1359" t="n">
-        <v>960.3180333333335</v>
+        <v>960.3180333333332</v>
       </c>
     </row>
     <row r="1360">
@@ -11325,7 +11325,7 @@
         <v>1360</v>
       </c>
       <c r="B1362" t="n">
-        <v>617.4561087301588</v>
+        <v>617.4561087301587</v>
       </c>
     </row>
     <row r="1363">
@@ -11333,7 +11333,7 @@
         <v>1361</v>
       </c>
       <c r="B1363" t="n">
-        <v>448.08825</v>
+        <v>448.0882500000001</v>
       </c>
     </row>
     <row r="1364">
@@ -11341,7 +11341,7 @@
         <v>1362</v>
       </c>
       <c r="B1364" t="n">
-        <v>827.15</v>
+        <v>827.1499999999999</v>
       </c>
     </row>
     <row r="1365">
@@ -11413,7 +11413,7 @@
         <v>1371</v>
       </c>
       <c r="B1373" t="n">
-        <v>307.0300833333332</v>
+        <v>307.0300833333333</v>
       </c>
     </row>
     <row r="1374">
@@ -11461,7 +11461,7 @@
         <v>1377</v>
       </c>
       <c r="B1379" t="n">
-        <v>331.2624999999999</v>
+        <v>331.2625</v>
       </c>
     </row>
     <row r="1380">
@@ -11477,7 +11477,7 @@
         <v>1379</v>
       </c>
       <c r="B1381" t="n">
-        <v>417.5011111111112</v>
+        <v>417.5011111111111</v>
       </c>
     </row>
     <row r="1382">
@@ -11493,7 +11493,7 @@
         <v>1381</v>
       </c>
       <c r="B1383" t="n">
-        <v>341.7833333333334</v>
+        <v>341.7833333333333</v>
       </c>
     </row>
     <row r="1384">
@@ -11573,7 +11573,7 @@
         <v>1391</v>
       </c>
       <c r="B1393" t="n">
-        <v>628.8516666666667</v>
+        <v>628.8516666666666</v>
       </c>
     </row>
     <row r="1394">
@@ -11733,7 +11733,7 @@
         <v>1411</v>
       </c>
       <c r="B1413" t="n">
-        <v>983.1904444444444</v>
+        <v>983.1904444444447</v>
       </c>
     </row>
     <row r="1414">
@@ -11741,7 +11741,7 @@
         <v>1412</v>
       </c>
       <c r="B1414" t="n">
-        <v>966.2743333333332</v>
+        <v>966.2743333333333</v>
       </c>
     </row>
     <row r="1415">
@@ -11757,7 +11757,7 @@
         <v>1414</v>
       </c>
       <c r="B1416" t="n">
-        <v>151.0225000000001</v>
+        <v>151.0225000000002</v>
       </c>
     </row>
     <row r="1417">
@@ -11869,7 +11869,7 @@
         <v>1428</v>
       </c>
       <c r="B1430" t="n">
-        <v>950.2582916666665</v>
+        <v>950.2582916666664</v>
       </c>
     </row>
     <row r="1431">
@@ -11893,7 +11893,7 @@
         <v>1431</v>
       </c>
       <c r="B1433" t="n">
-        <v>267.2425555555556</v>
+        <v>267.2425555555557</v>
       </c>
     </row>
     <row r="1434">
@@ -11981,7 +11981,7 @@
         <v>1442</v>
       </c>
       <c r="B1444" t="n">
-        <v>494.2466666666666</v>
+        <v>494.2466666666667</v>
       </c>
     </row>
     <row r="1445">
@@ -11989,7 +11989,7 @@
         <v>1443</v>
       </c>
       <c r="B1445" t="n">
-        <v>1410.909666666666</v>
+        <v>1410.909666666667</v>
       </c>
     </row>
     <row r="1446">
@@ -12013,7 +12013,7 @@
         <v>1446</v>
       </c>
       <c r="B1448" t="n">
-        <v>578.4888888888889</v>
+        <v>578.4888888888888</v>
       </c>
     </row>
     <row r="1449">
@@ -12029,7 +12029,7 @@
         <v>1448</v>
       </c>
       <c r="B1450" t="n">
-        <v>225.846976190476</v>
+        <v>225.8469761904761</v>
       </c>
     </row>
     <row r="1451">
@@ -12205,7 +12205,7 @@
         <v>1470</v>
       </c>
       <c r="B1472" t="n">
-        <v>400.7765555555556</v>
+        <v>400.7765555555557</v>
       </c>
     </row>
     <row r="1473">
@@ -12269,7 +12269,7 @@
         <v>1478</v>
       </c>
       <c r="B1480" t="n">
-        <v>449.1395</v>
+        <v>449.1394999999999</v>
       </c>
     </row>
     <row r="1481">
@@ -12285,7 +12285,7 @@
         <v>1480</v>
       </c>
       <c r="B1482" t="n">
-        <v>831.8629999999998</v>
+        <v>831.8629999999999</v>
       </c>
     </row>
     <row r="1483">
@@ -12317,7 +12317,7 @@
         <v>1484</v>
       </c>
       <c r="B1486" t="n">
-        <v>526.4930000000001</v>
+        <v>526.4929999999999</v>
       </c>
     </row>
     <row r="1487">
@@ -12325,7 +12325,7 @@
         <v>1485</v>
       </c>
       <c r="B1487" t="n">
-        <v>617.4561087301588</v>
+        <v>617.4561087301587</v>
       </c>
     </row>
     <row r="1488">
@@ -12333,7 +12333,7 @@
         <v>1486</v>
       </c>
       <c r="B1488" t="n">
-        <v>757.3666666666667</v>
+        <v>757.3666666666666</v>
       </c>
     </row>
     <row r="1489">
@@ -12389,7 +12389,7 @@
         <v>1493</v>
       </c>
       <c r="B1495" t="n">
-        <v>774.0946666666666</v>
+        <v>774.0946666666667</v>
       </c>
     </row>
     <row r="1496">
@@ -12557,7 +12557,7 @@
         <v>1514</v>
       </c>
       <c r="B1516" t="n">
-        <v>332.8166666666667</v>
+        <v>332.8166666666666</v>
       </c>
     </row>
     <row r="1517">
@@ -12573,7 +12573,7 @@
         <v>1516</v>
       </c>
       <c r="B1518" t="n">
-        <v>283.3553333333332</v>
+        <v>283.3553333333333</v>
       </c>
     </row>
     <row r="1519">
@@ -12629,7 +12629,7 @@
         <v>1523</v>
       </c>
       <c r="B1525" t="n">
-        <v>367.8499999999999</v>
+        <v>367.85</v>
       </c>
     </row>
     <row r="1526">
@@ -12725,7 +12725,7 @@
         <v>1535</v>
       </c>
       <c r="B1537" t="n">
-        <v>725.6652380952382</v>
+        <v>725.6652380952381</v>
       </c>
     </row>
     <row r="1538">
@@ -12901,7 +12901,7 @@
         <v>1557</v>
       </c>
       <c r="B1559" t="n">
-        <v>321.7978095238095</v>
+        <v>321.7978095238096</v>
       </c>
     </row>
     <row r="1560">

</xml_diff>